<commit_message>
Change the pretrained model used in the paper.
</commit_message>
<xml_diff>
--- a/TestingResult/McMaster/McMaster_cpsnr_crop_0_ignore_5.xlsx
+++ b/TestingResult/McMaster/McMaster_cpsnr_crop_0_ignore_5.xlsx
@@ -431,16 +431,16 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>28.87426567077637</v>
+        <v>28.94093322753906</v>
       </c>
       <c r="C1" t="n">
-        <v>31.67053413391113</v>
+        <v>31.72183799743652</v>
       </c>
       <c r="D1" t="n">
-        <v>27.08889007568359</v>
+        <v>27.09791946411133</v>
       </c>
       <c r="E1" t="n">
-        <v>28.82570648193359</v>
+        <v>28.86097145080566</v>
       </c>
     </row>
     <row r="2">
@@ -450,16 +450,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>38.10578918457031</v>
+        <v>38.1544075012207</v>
       </c>
       <c r="C2" t="n">
-        <v>41.21038436889648</v>
+        <v>41.35848236083984</v>
       </c>
       <c r="D2" t="n">
-        <v>36.97233200073242</v>
+        <v>37.01863098144531</v>
       </c>
       <c r="E2" t="n">
-        <v>38.42489624023438</v>
+        <v>38.48972320556641</v>
       </c>
     </row>
     <row r="3">
@@ -469,16 +469,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>39.20629119873047</v>
+        <v>39.22373199462891</v>
       </c>
       <c r="C3" t="n">
-        <v>41.14473342895508</v>
+        <v>41.19161605834961</v>
       </c>
       <c r="D3" t="n">
-        <v>38.11057281494141</v>
+        <v>38.12992858886719</v>
       </c>
       <c r="E3" t="n">
-        <v>39.31336212158203</v>
+        <v>39.33806228637695</v>
       </c>
     </row>
     <row r="4">
@@ -488,16 +488,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38.52389907836914</v>
+        <v>38.71438598632812</v>
       </c>
       <c r="C4" t="n">
-        <v>41.67699813842773</v>
+        <v>41.70479202270508</v>
       </c>
       <c r="D4" t="n">
-        <v>38.08890914916992</v>
+        <v>38.06488418579102</v>
       </c>
       <c r="E4" t="n">
-        <v>39.16349792480469</v>
+        <v>39.23088836669922</v>
       </c>
     </row>
     <row r="5">
@@ -507,16 +507,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>41.68989562988281</v>
+        <v>41.78150939941406</v>
       </c>
       <c r="C5" t="n">
-        <v>44.21748352050781</v>
+        <v>44.35115051269531</v>
       </c>
       <c r="D5" t="n">
-        <v>38.57791137695312</v>
+        <v>38.58174133300781</v>
       </c>
       <c r="E5" t="n">
-        <v>40.89065551757812</v>
+        <v>40.93862533569336</v>
       </c>
     </row>
     <row r="6">
@@ -526,16 +526,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>39.33166885375977</v>
+        <v>39.36916351318359</v>
       </c>
       <c r="C6" t="n">
-        <v>42.73376846313477</v>
+        <v>42.84889602661133</v>
       </c>
       <c r="D6" t="n">
-        <v>36.47513198852539</v>
+        <v>36.46199035644531</v>
       </c>
       <c r="E6" t="n">
-        <v>38.80435180664062</v>
+        <v>38.82323837280273</v>
       </c>
     </row>
     <row r="7">
@@ -545,16 +545,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>37.35624694824219</v>
+        <v>37.40185546875</v>
       </c>
       <c r="C7" t="n">
-        <v>42.29444885253906</v>
+        <v>42.38032913208008</v>
       </c>
       <c r="D7" t="n">
-        <v>39.1088981628418</v>
+        <v>39.09905242919922</v>
       </c>
       <c r="E7" t="n">
-        <v>39.14178085327148</v>
+        <v>39.17512512207031</v>
       </c>
     </row>
     <row r="8">
@@ -564,16 +564,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>33.36825180053711</v>
+        <v>33.43342208862305</v>
       </c>
       <c r="C8" t="n">
-        <v>34.10794067382812</v>
+        <v>34.10016632080078</v>
       </c>
       <c r="D8" t="n">
-        <v>32.56278610229492</v>
+        <v>32.573974609375</v>
       </c>
       <c r="E8" t="n">
-        <v>33.30049133300781</v>
+        <v>33.32404708862305</v>
       </c>
     </row>
     <row r="9">
@@ -583,16 +583,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31.94231414794922</v>
+        <v>32.00667190551758</v>
       </c>
       <c r="C9" t="n">
-        <v>34.88896179199219</v>
+        <v>35.03984832763672</v>
       </c>
       <c r="D9" t="n">
-        <v>31.05270385742188</v>
+        <v>31.15790939331055</v>
       </c>
       <c r="E9" t="n">
-        <v>32.34441375732422</v>
+        <v>32.44304656982422</v>
       </c>
     </row>
     <row r="10">
@@ -602,16 +602,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>34.66515350341797</v>
+        <v>34.69312286376953</v>
       </c>
       <c r="C10" t="n">
-        <v>37.13493728637695</v>
+        <v>37.1483268737793</v>
       </c>
       <c r="D10" t="n">
-        <v>35.03449249267578</v>
+        <v>35.09734725952148</v>
       </c>
       <c r="E10" t="n">
-        <v>35.48355865478516</v>
+        <v>35.52105331420898</v>
       </c>
     </row>
     <row r="11">
@@ -621,16 +621,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>34.49716186523438</v>
+        <v>34.56444549560547</v>
       </c>
       <c r="C11" t="n">
-        <v>38.62919998168945</v>
+        <v>38.73139190673828</v>
       </c>
       <c r="D11" t="n">
-        <v>32.90534210205078</v>
+        <v>32.91348266601562</v>
       </c>
       <c r="E11" t="n">
-        <v>34.75218963623047</v>
+        <v>34.79392623901367</v>
       </c>
     </row>
     <row r="12">
@@ -640,16 +640,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>34.69091796875</v>
+        <v>34.70332717895508</v>
       </c>
       <c r="C12" t="n">
-        <v>37.03701400756836</v>
+        <v>37.11955642700195</v>
       </c>
       <c r="D12" t="n">
-        <v>32.0632209777832</v>
+        <v>32.11446380615234</v>
       </c>
       <c r="E12" t="n">
-        <v>34.12953186035156</v>
+        <v>34.17467880249023</v>
       </c>
     </row>
     <row r="13">
@@ -659,16 +659,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>36.20252990722656</v>
+        <v>36.15987777709961</v>
       </c>
       <c r="C13" t="n">
-        <v>39.14806747436523</v>
+        <v>39.22965621948242</v>
       </c>
       <c r="D13" t="n">
-        <v>34.52121353149414</v>
+        <v>34.58393096923828</v>
       </c>
       <c r="E13" t="n">
-        <v>36.23118591308594</v>
+        <v>36.26144027709961</v>
       </c>
     </row>
     <row r="14">
@@ -678,16 +678,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>35.5900993347168</v>
+        <v>35.70352935791016</v>
       </c>
       <c r="C14" t="n">
-        <v>37.75800323486328</v>
+        <v>37.88385772705078</v>
       </c>
       <c r="D14" t="n">
-        <v>31.81171035766602</v>
+        <v>31.85197448730469</v>
       </c>
       <c r="E14" t="n">
-        <v>34.34728240966797</v>
+        <v>34.418701171875</v>
       </c>
     </row>
     <row r="15">
@@ -697,16 +697,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>38.48916244506836</v>
+        <v>38.61904144287109</v>
       </c>
       <c r="C15" t="n">
-        <v>40.70053100585938</v>
+        <v>40.88594436645508</v>
       </c>
       <c r="D15" t="n">
-        <v>35.27649688720703</v>
+        <v>35.36655807495117</v>
       </c>
       <c r="E15" t="n">
-        <v>37.58260345458984</v>
+        <v>37.69879913330078</v>
       </c>
     </row>
     <row r="16">
@@ -716,16 +716,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>40.77238464355469</v>
+        <v>40.76079940795898</v>
       </c>
       <c r="C16" t="n">
-        <v>43.9008903503418</v>
+        <v>43.88357162475586</v>
       </c>
       <c r="D16" t="n">
-        <v>39.02083587646484</v>
+        <v>39.00116348266602</v>
       </c>
       <c r="E16" t="n">
-        <v>40.79656600952148</v>
+        <v>40.77998352050781</v>
       </c>
     </row>
     <row r="17">
@@ -735,16 +735,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>39.03805160522461</v>
+        <v>39.04787445068359</v>
       </c>
       <c r="C17" t="n">
-        <v>42.85449600219727</v>
+        <v>42.90390396118164</v>
       </c>
       <c r="D17" t="n">
-        <v>38.74518203735352</v>
+        <v>38.77669525146484</v>
       </c>
       <c r="E17" t="n">
-        <v>39.85590362548828</v>
+        <v>39.88165664672852</v>
       </c>
     </row>
     <row r="18">
@@ -754,16 +754,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>36.29069900512695</v>
+        <v>36.29543304443359</v>
       </c>
       <c r="C18" t="n">
-        <v>40.41513061523438</v>
+        <v>40.55448913574219</v>
       </c>
       <c r="D18" t="n">
-        <v>36.48628234863281</v>
+        <v>36.54620742797852</v>
       </c>
       <c r="E18" t="n">
-        <v>37.36450576782227</v>
+        <v>37.41373443603516</v>
       </c>
     </row>
     <row r="19">
@@ -773,16 +773,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>36.59082126617432</v>
+        <v>36.64297400580512</v>
       </c>
       <c r="C19" t="n">
-        <v>39.5290846294827</v>
+        <v>39.61321205563016</v>
       </c>
       <c r="D19" t="n">
-        <v>35.21682845221626</v>
+        <v>35.24654748704698</v>
       </c>
       <c r="E19" t="n">
-        <v>36.70847129821777</v>
+        <v>36.75376118554009</v>
       </c>
     </row>
   </sheetData>
@@ -811,16 +811,16 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>29.91922187805176</v>
+        <v>29.96093368530273</v>
       </c>
       <c r="C1" t="n">
-        <v>32.36798095703125</v>
+        <v>32.40523529052734</v>
       </c>
       <c r="D1" t="n">
-        <v>27.63231658935547</v>
+        <v>27.6295108795166</v>
       </c>
       <c r="E1" t="n">
-        <v>29.55539894104004</v>
+        <v>29.57317352294922</v>
       </c>
     </row>
     <row r="2">
@@ -830,16 +830,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>39.02953720092773</v>
+        <v>39.12648010253906</v>
       </c>
       <c r="C2" t="n">
-        <v>41.93213653564453</v>
+        <v>42.06500625610352</v>
       </c>
       <c r="D2" t="n">
-        <v>37.6004753112793</v>
+        <v>37.65140151977539</v>
       </c>
       <c r="E2" t="n">
-        <v>39.17346572875977</v>
+        <v>39.25460433959961</v>
       </c>
     </row>
     <row r="3">
@@ -849,16 +849,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40.23498153686523</v>
+        <v>40.30384826660156</v>
       </c>
       <c r="C3" t="n">
-        <v>41.90366744995117</v>
+        <v>41.93997192382812</v>
       </c>
       <c r="D3" t="n">
-        <v>38.89986801147461</v>
+        <v>38.93620300292969</v>
       </c>
       <c r="E3" t="n">
-        <v>40.17618560791016</v>
+        <v>40.22319030761719</v>
       </c>
     </row>
     <row r="4">
@@ -868,16 +868,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>39.72566986083984</v>
+        <v>39.92569732666016</v>
       </c>
       <c r="C4" t="n">
-        <v>42.00288391113281</v>
+        <v>41.97026062011719</v>
       </c>
       <c r="D4" t="n">
-        <v>38.34249114990234</v>
+        <v>38.30780029296875</v>
       </c>
       <c r="E4" t="n">
-        <v>39.77371978759766</v>
+        <v>39.81715393066406</v>
       </c>
     </row>
     <row r="5">
@@ -887,16 +887,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>42.95400619506836</v>
+        <v>43.04160308837891</v>
       </c>
       <c r="C5" t="n">
-        <v>44.84104156494141</v>
+        <v>44.98368835449219</v>
       </c>
       <c r="D5" t="n">
-        <v>38.78401947021484</v>
+        <v>38.7957649230957</v>
       </c>
       <c r="E5" t="n">
-        <v>41.43138885498047</v>
+        <v>41.48055267333984</v>
       </c>
     </row>
     <row r="6">
@@ -906,16 +906,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>39.85243988037109</v>
+        <v>39.93154907226562</v>
       </c>
       <c r="C6" t="n">
-        <v>43.22993469238281</v>
+        <v>43.31013488769531</v>
       </c>
       <c r="D6" t="n">
-        <v>36.76100921630859</v>
+        <v>36.78837966918945</v>
       </c>
       <c r="E6" t="n">
-        <v>39.18647384643555</v>
+        <v>39.23550796508789</v>
       </c>
     </row>
     <row r="7">
@@ -925,16 +925,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>37.74883651733398</v>
+        <v>37.87023162841797</v>
       </c>
       <c r="C7" t="n">
-        <v>42.52582931518555</v>
+        <v>42.66083526611328</v>
       </c>
       <c r="D7" t="n">
-        <v>39.41323852539062</v>
+        <v>39.47819900512695</v>
       </c>
       <c r="E7" t="n">
-        <v>39.47829818725586</v>
+        <v>39.58274841308594</v>
       </c>
     </row>
     <row r="8">
@@ -944,16 +944,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>34.67374801635742</v>
+        <v>34.73881530761719</v>
       </c>
       <c r="C8" t="n">
-        <v>34.82109451293945</v>
+        <v>34.83522415161133</v>
       </c>
       <c r="D8" t="n">
-        <v>33.97643280029297</v>
+        <v>34.00452423095703</v>
       </c>
       <c r="E8" t="n">
-        <v>34.47454071044922</v>
+        <v>34.51005554199219</v>
       </c>
     </row>
     <row r="9">
@@ -963,16 +963,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>33.15036010742188</v>
+        <v>33.23057556152344</v>
       </c>
       <c r="C9" t="n">
-        <v>36.23389053344727</v>
+        <v>36.39508819580078</v>
       </c>
       <c r="D9" t="n">
-        <v>32.30916595458984</v>
+        <v>32.36769485473633</v>
       </c>
       <c r="E9" t="n">
-        <v>33.59931564331055</v>
+        <v>33.68436431884766</v>
       </c>
     </row>
     <row r="10">
@@ -982,16 +982,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>35.03701782226562</v>
+        <v>35.08209609985352</v>
       </c>
       <c r="C10" t="n">
-        <v>37.20601654052734</v>
+        <v>37.21687698364258</v>
       </c>
       <c r="D10" t="n">
-        <v>36.27607727050781</v>
+        <v>36.34161758422852</v>
       </c>
       <c r="E10" t="n">
-        <v>36.08157348632812</v>
+        <v>36.12432098388672</v>
       </c>
     </row>
     <row r="11">
@@ -1001,16 +1001,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>35.13019943237305</v>
+        <v>35.18029403686523</v>
       </c>
       <c r="C11" t="n">
-        <v>39.269287109375</v>
+        <v>39.3519172668457</v>
       </c>
       <c r="D11" t="n">
-        <v>33.2667236328125</v>
+        <v>33.29235458374023</v>
       </c>
       <c r="E11" t="n">
-        <v>35.2454948425293</v>
+        <v>35.2869758605957</v>
       </c>
     </row>
     <row r="12">
@@ -1020,16 +1020,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>35.35680770874023</v>
+        <v>35.36347198486328</v>
       </c>
       <c r="C12" t="n">
-        <v>37.64036560058594</v>
+        <v>37.71631622314453</v>
       </c>
       <c r="D12" t="n">
-        <v>32.5984992980957</v>
+        <v>32.61042785644531</v>
       </c>
       <c r="E12" t="n">
-        <v>34.71430587768555</v>
+        <v>34.73553085327148</v>
       </c>
     </row>
     <row r="13">
@@ -1039,16 +1039,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>38.08137893676758</v>
+        <v>38.11630249023438</v>
       </c>
       <c r="C13" t="n">
-        <v>40.74541473388672</v>
+        <v>40.9373779296875</v>
       </c>
       <c r="D13" t="n">
-        <v>35.39481735229492</v>
+        <v>35.44962310791016</v>
       </c>
       <c r="E13" t="n">
-        <v>37.54057312011719</v>
+        <v>37.61105728149414</v>
       </c>
     </row>
     <row r="14">
@@ -1058,16 +1058,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>36.90947341918945</v>
+        <v>36.99066543579102</v>
       </c>
       <c r="C14" t="n">
-        <v>38.41114807128906</v>
+        <v>38.53049468994141</v>
       </c>
       <c r="D14" t="n">
-        <v>32.21348190307617</v>
+        <v>32.24367523193359</v>
       </c>
       <c r="E14" t="n">
-        <v>35.00041198730469</v>
+        <v>35.05496978759766</v>
       </c>
     </row>
     <row r="15">
@@ -1077,16 +1077,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>39.43158340454102</v>
+        <v>39.52053451538086</v>
       </c>
       <c r="C15" t="n">
-        <v>42.04677200317383</v>
+        <v>42.23884582519531</v>
       </c>
       <c r="D15" t="n">
-        <v>36.48725891113281</v>
+        <v>36.53905487060547</v>
       </c>
       <c r="E15" t="n">
-        <v>38.74049377441406</v>
+        <v>38.82441711425781</v>
       </c>
     </row>
     <row r="16">
@@ -1096,16 +1096,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>41.33487319946289</v>
+        <v>41.37936019897461</v>
       </c>
       <c r="C16" t="n">
-        <v>44.41224670410156</v>
+        <v>44.41862487792969</v>
       </c>
       <c r="D16" t="n">
-        <v>39.66964721679688</v>
+        <v>39.55954360961914</v>
       </c>
       <c r="E16" t="n">
-        <v>41.39368438720703</v>
+        <v>41.35459136962891</v>
       </c>
     </row>
     <row r="17">
@@ -1115,16 +1115,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>39.30684661865234</v>
+        <v>39.290771484375</v>
       </c>
       <c r="C17" t="n">
-        <v>43.19620513916016</v>
+        <v>43.25550079345703</v>
       </c>
       <c r="D17" t="n">
-        <v>39.12596130371094</v>
+        <v>39.14389038085938</v>
       </c>
       <c r="E17" t="n">
-        <v>40.18478393554688</v>
+        <v>40.19565582275391</v>
       </c>
     </row>
     <row r="18">
@@ -1134,16 +1134,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>36.98008346557617</v>
+        <v>36.98944854736328</v>
       </c>
       <c r="C18" t="n">
-        <v>41.26882171630859</v>
+        <v>41.38068771362305</v>
       </c>
       <c r="D18" t="n">
-        <v>37.04816055297852</v>
+        <v>37.08298110961914</v>
       </c>
       <c r="E18" t="n">
-        <v>38.02779769897461</v>
+        <v>38.0638542175293</v>
       </c>
     </row>
     <row r="19">
@@ -1153,16 +1153,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>37.49205917782254</v>
+        <v>37.55792660183377</v>
       </c>
       <c r="C19" t="n">
-        <v>40.2252631717258</v>
+        <v>40.31178262498644</v>
       </c>
       <c r="D19" t="n">
-        <v>35.87775802612305</v>
+        <v>35.90125815073649</v>
       </c>
       <c r="E19" t="n">
-        <v>37.43210591210259</v>
+        <v>37.47848468356662</v>
       </c>
     </row>
   </sheetData>
@@ -1191,16 +1191,16 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>30.29011917114258</v>
+        <v>30.35678672790527</v>
       </c>
       <c r="C1" t="n">
-        <v>32.61494064331055</v>
+        <v>32.67437362670898</v>
       </c>
       <c r="D1" t="n">
-        <v>28.15296363830566</v>
+        <v>28.15261459350586</v>
       </c>
       <c r="E1" t="n">
-        <v>29.98110961914062</v>
+        <v>30.0123119354248</v>
       </c>
     </row>
     <row r="2">
@@ -1210,16 +1210,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>39.50413131713867</v>
+        <v>39.61936187744141</v>
       </c>
       <c r="C2" t="n">
-        <v>42.36390686035156</v>
+        <v>42.48798370361328</v>
       </c>
       <c r="D2" t="n">
-        <v>37.98130416870117</v>
+        <v>38.03919982910156</v>
       </c>
       <c r="E2" t="n">
-        <v>39.59539413452148</v>
+        <v>39.68436813354492</v>
       </c>
     </row>
     <row r="3">
@@ -1229,16 +1229,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40.68164825439453</v>
+        <v>40.73922729492188</v>
       </c>
       <c r="C3" t="n">
-        <v>42.24077606201172</v>
+        <v>42.28229522705078</v>
       </c>
       <c r="D3" t="n">
-        <v>39.29452514648438</v>
+        <v>39.34452819824219</v>
       </c>
       <c r="E3" t="n">
-        <v>40.57487487792969</v>
+        <v>40.62541198730469</v>
       </c>
     </row>
     <row r="4">
@@ -1248,16 +1248,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40.12480163574219</v>
+        <v>40.34889221191406</v>
       </c>
       <c r="C4" t="n">
-        <v>42.54238891601562</v>
+        <v>42.51802825927734</v>
       </c>
       <c r="D4" t="n">
-        <v>38.65119552612305</v>
+        <v>38.64346313476562</v>
       </c>
       <c r="E4" t="n">
-        <v>40.15808486938477</v>
+        <v>40.22359466552734</v>
       </c>
     </row>
     <row r="5">
@@ -1267,16 +1267,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>43.30990219116211</v>
+        <v>43.42312622070312</v>
       </c>
       <c r="C5" t="n">
-        <v>45.30385971069336</v>
+        <v>45.37884521484375</v>
       </c>
       <c r="D5" t="n">
-        <v>38.9868278503418</v>
+        <v>39.0314826965332</v>
       </c>
       <c r="E5" t="n">
-        <v>41.7085075378418</v>
+        <v>41.77330017089844</v>
       </c>
     </row>
     <row r="6">
@@ -1286,16 +1286,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>40.23293304443359</v>
+        <v>40.30735397338867</v>
       </c>
       <c r="C6" t="n">
-        <v>43.53156661987305</v>
+        <v>43.636962890625</v>
       </c>
       <c r="D6" t="n">
-        <v>36.97597122192383</v>
+        <v>37.04833602905273</v>
       </c>
       <c r="E6" t="n">
-        <v>39.45954132080078</v>
+        <v>39.53677749633789</v>
       </c>
     </row>
     <row r="7">
@@ -1305,16 +1305,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>38.06668090820312</v>
+        <v>38.21192932128906</v>
       </c>
       <c r="C7" t="n">
-        <v>42.80032348632812</v>
+        <v>42.98377227783203</v>
       </c>
       <c r="D7" t="n">
-        <v>39.63575744628906</v>
+        <v>39.72381210327148</v>
       </c>
       <c r="E7" t="n">
-        <v>39.75650787353516</v>
+        <v>39.88833618164062</v>
       </c>
     </row>
     <row r="8">
@@ -1324,16 +1324,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>35.31167602539062</v>
+        <v>35.38027572631836</v>
       </c>
       <c r="C8" t="n">
-        <v>35.29892730712891</v>
+        <v>35.30629730224609</v>
       </c>
       <c r="D8" t="n">
-        <v>34.46769332885742</v>
+        <v>34.50374984741211</v>
       </c>
       <c r="E8" t="n">
-        <v>35.00778198242188</v>
+        <v>35.04494094848633</v>
       </c>
     </row>
     <row r="9">
@@ -1343,16 +1343,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>33.84683227539062</v>
+        <v>33.89922714233398</v>
       </c>
       <c r="C9" t="n">
-        <v>36.95016479492188</v>
+        <v>37.08980941772461</v>
       </c>
       <c r="D9" t="n">
-        <v>32.86042022705078</v>
+        <v>32.94660186767578</v>
       </c>
       <c r="E9" t="n">
-        <v>34.23357772827148</v>
+        <v>34.31687545776367</v>
       </c>
     </row>
     <row r="10">
@@ -1362,16 +1362,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>35.50553131103516</v>
+        <v>35.56650924682617</v>
       </c>
       <c r="C10" t="n">
-        <v>37.50531387329102</v>
+        <v>37.503173828125</v>
       </c>
       <c r="D10" t="n">
-        <v>37.23382186889648</v>
+        <v>37.33901596069336</v>
       </c>
       <c r="E10" t="n">
-        <v>36.65440368652344</v>
+        <v>36.71079254150391</v>
       </c>
     </row>
     <row r="11">
@@ -1381,16 +1381,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>35.44861221313477</v>
+        <v>35.50518417358398</v>
       </c>
       <c r="C11" t="n">
-        <v>39.51646423339844</v>
+        <v>39.59118270874023</v>
       </c>
       <c r="D11" t="n">
-        <v>33.4652214050293</v>
+        <v>33.50859069824219</v>
       </c>
       <c r="E11" t="n">
-        <v>35.49111938476562</v>
+        <v>35.54305648803711</v>
       </c>
     </row>
     <row r="12">
@@ -1400,16 +1400,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>35.78126525878906</v>
+        <v>35.80410766601562</v>
       </c>
       <c r="C12" t="n">
-        <v>37.97463226318359</v>
+        <v>38.03202056884766</v>
       </c>
       <c r="D12" t="n">
-        <v>32.96611022949219</v>
+        <v>32.95048141479492</v>
       </c>
       <c r="E12" t="n">
-        <v>35.09248352050781</v>
+        <v>35.10023880004883</v>
       </c>
     </row>
     <row r="13">
@@ -1419,16 +1419,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>38.78005218505859</v>
+        <v>38.86020660400391</v>
       </c>
       <c r="C13" t="n">
-        <v>41.66530990600586</v>
+        <v>41.84979248046875</v>
       </c>
       <c r="D13" t="n">
-        <v>35.98110580444336</v>
+        <v>35.99428176879883</v>
       </c>
       <c r="E13" t="n">
-        <v>38.21150970458984</v>
+        <v>38.26963043212891</v>
       </c>
     </row>
     <row r="14">
@@ -1438,16 +1438,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>37.21125411987305</v>
+        <v>37.35730361938477</v>
       </c>
       <c r="C14" t="n">
-        <v>38.80447769165039</v>
+        <v>38.91839981079102</v>
       </c>
       <c r="D14" t="n">
-        <v>32.64206695556641</v>
+        <v>32.68972778320312</v>
       </c>
       <c r="E14" t="n">
-        <v>35.39610290527344</v>
+        <v>35.47522735595703</v>
       </c>
     </row>
     <row r="15">
@@ -1457,16 +1457,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>40.03837585449219</v>
+        <v>40.13093948364258</v>
       </c>
       <c r="C15" t="n">
-        <v>42.80202484130859</v>
+        <v>42.92842483520508</v>
       </c>
       <c r="D15" t="n">
-        <v>36.97260284423828</v>
+        <v>37.02784729003906</v>
       </c>
       <c r="E15" t="n">
-        <v>39.30127716064453</v>
+        <v>39.37753295898438</v>
       </c>
     </row>
     <row r="16">
@@ -1476,16 +1476,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>41.57543563842773</v>
+        <v>41.68775939941406</v>
       </c>
       <c r="C16" t="n">
-        <v>44.65888214111328</v>
+        <v>44.73407363891602</v>
       </c>
       <c r="D16" t="n">
-        <v>40.11274337768555</v>
+        <v>40.01743698120117</v>
       </c>
       <c r="E16" t="n">
-        <v>41.7345085144043</v>
+        <v>41.73886108398438</v>
       </c>
     </row>
     <row r="17">
@@ -1495,16 +1495,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>39.37554168701172</v>
+        <v>39.39449310302734</v>
       </c>
       <c r="C17" t="n">
-        <v>43.51191711425781</v>
+        <v>43.57820892333984</v>
       </c>
       <c r="D17" t="n">
-        <v>39.47352600097656</v>
+        <v>39.50307846069336</v>
       </c>
       <c r="E17" t="n">
-        <v>40.41121673583984</v>
+        <v>40.44224548339844</v>
       </c>
     </row>
     <row r="18">
@@ -1514,16 +1514,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>37.56850433349609</v>
+        <v>37.60507965087891</v>
       </c>
       <c r="C18" t="n">
-        <v>41.76287841796875</v>
+        <v>41.86933517456055</v>
       </c>
       <c r="D18" t="n">
-        <v>37.39557647705078</v>
+        <v>37.43199157714844</v>
       </c>
       <c r="E18" t="n">
-        <v>38.49921798706055</v>
+        <v>38.5466423034668</v>
       </c>
     </row>
     <row r="19">
@@ -1533,16 +1533,16 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>37.9251831902398</v>
+        <v>38.01098685794406</v>
       </c>
       <c r="C19" t="n">
-        <v>40.65826416015625</v>
+        <v>40.74238777160645</v>
       </c>
       <c r="D19" t="n">
-        <v>36.29163519541422</v>
+        <v>36.32756890190972</v>
       </c>
       <c r="E19" t="n">
-        <v>37.84817886352539</v>
+        <v>37.90611913469102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>